<commit_message>
Incorporating EPV sequences from DIGS and EPV refseqs
</commit_message>
<xml_diff>
--- a/tabular/genus/dependo-refseqs-side-data.xlsx
+++ b/tabular/genus/dependo-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10913"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/AAV-GLUE/tabular/genus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87B8951-537C-F246-B851-3CC1FE1C9936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CF1CC9-B8AE-C040-AF24-1975D2781A83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1300" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="125">
   <si>
     <t>accession-ID</t>
   </si>
@@ -2717,10 +2717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="A1:M32"/>
+      <selection activeCell="I30" sqref="A1:L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2734,10 +2734,9 @@
     <col min="10" max="10" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="26.83203125" customWidth="1"/>
     <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2774,11 +2773,8 @@
       <c r="L1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>41</v>
       </c>
@@ -2815,11 +2811,8 @@
       <c r="L2" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
@@ -2856,11 +2849,8 @@
       <c r="L3" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>9</v>
       </c>
@@ -2897,11 +2887,8 @@
       <c r="L4" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="9" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -2938,11 +2925,8 @@
       <c r="L5" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="M5" s="9" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>84</v>
       </c>
@@ -2977,11 +2961,8 @@
       <c r="L6" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="M6" s="9" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>86</v>
       </c>
@@ -3016,11 +2997,8 @@
       <c r="L7" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="M7" s="9" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>89</v>
       </c>
@@ -3055,11 +3033,8 @@
       <c r="L8" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="M8" s="9" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>88</v>
       </c>
@@ -3094,11 +3069,8 @@
       <c r="L9" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M9" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>87</v>
       </c>
@@ -3133,11 +3105,8 @@
       <c r="L10" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M10" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
@@ -3174,11 +3143,8 @@
       <c r="L11" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M11" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
@@ -3215,11 +3181,8 @@
       <c r="L12" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M12" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>31</v>
       </c>
@@ -3256,11 +3219,8 @@
       <c r="L13" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M13" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
@@ -3297,11 +3257,8 @@
       <c r="L14" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M14" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>4</v>
       </c>
@@ -3338,11 +3295,8 @@
       <c r="L15" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M15" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
@@ -3379,11 +3333,8 @@
       <c r="L16" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M16" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
@@ -3420,11 +3371,8 @@
       <c r="L17" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M17" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
@@ -3461,11 +3409,8 @@
       <c r="L18" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M18" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
@@ -3502,11 +3447,8 @@
       <c r="L19" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M19" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
@@ -3543,11 +3485,8 @@
       <c r="L20" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M20" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>40</v>
       </c>
@@ -3584,11 +3523,8 @@
       <c r="L21" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M21" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>27</v>
       </c>
@@ -3625,11 +3561,8 @@
       <c r="L22" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M22" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
@@ -3666,11 +3599,8 @@
       <c r="L23" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M23" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -3707,11 +3637,8 @@
       <c r="L24" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M24" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>28</v>
       </c>
@@ -3748,11 +3675,8 @@
       <c r="L25" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M25" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>33</v>
       </c>
@@ -3789,11 +3713,8 @@
       <c r="L26" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M26" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>7</v>
       </c>
@@ -3830,11 +3751,8 @@
       <c r="L27" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M27" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>38</v>
       </c>
@@ -3871,11 +3789,8 @@
       <c r="L28" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M28" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>85</v>
       </c>
@@ -3910,11 +3825,8 @@
       <c r="L29" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M29" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
         <v>104</v>
       </c>
@@ -3951,11 +3863,8 @@
       <c r="L30" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M30" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>78</v>
       </c>
@@ -3992,11 +3901,8 @@
       <c r="L31" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M31" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>79</v>
       </c>
@@ -4033,12 +3939,9 @@
       <c r="L32" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="M32" s="7" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M32">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L32">
     <sortCondition ref="H2:H32"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>